<commit_message>
quote generation for gateway
Former-commit-id: 73b4050cd0969b8a0e6fbf7210269a2d9a15203a
</commit_message>
<xml_diff>
--- a/db/dummydata/gateway/gateway__local_charges.xlsx
+++ b/db/dummydata/gateway/gateway__local_charges.xlsx
@@ -11,12 +11,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="81">
   <si>
     <t>EFFECTIVE_DATE</t>
   </si>
   <si>
     <t>EXPIRATION_DATE</t>
+  </si>
+  <si>
+    <t>CARRIER</t>
   </si>
   <si>
     <t>DESTINATION</t>
@@ -337,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -345,10 +348,10 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -367,6 +370,9 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -412,8 +418,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="5" width="26.57"/>
-    <col customWidth="1" min="11" max="11" width="16.86"/>
+    <col customWidth="1" min="1" max="6" width="26.57"/>
+    <col customWidth="1" min="12" max="12" width="16.86"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -429,7 +435,7 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -489,28 +495,29 @@
       <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="4"/>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="Z1" s="4"/>
       <c r="AA1" s="4"/>
       <c r="AB1" s="4"/>
       <c r="AC1" s="4"/>
       <c r="AD1" s="4"/>
+      <c r="AE1" s="4"/>
     </row>
     <row r="2">
       <c r="A2" s="5">
         <f t="shared" ref="A2:A37" si="1">TODAY()</f>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B2" s="5">
         <f t="shared" ref="B2:B37" si="2">A2+365</f>
-        <v>43672</v>
+        <v>43693</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
-      <c r="E2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="7" t="s">
         <v>25</v>
       </c>
       <c r="G2" s="6" t="s">
@@ -528,32 +535,33 @@
       <c r="K2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" s="6">
+      <c r="L2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R2" s="6">
         <v>4.5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B3" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
+        <v>43693</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
-      <c r="E3" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>25</v>
+      <c r="E3" s="6"/>
+      <c r="F3" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>28</v>
@@ -564,32 +572,33 @@
       <c r="K3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q3" s="6">
+      <c r="L3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R3" s="6">
         <v>2.5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B4" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
+        <v>43693</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
-      <c r="E4" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>25</v>
+      <c r="E4" s="6"/>
+      <c r="F4" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>28</v>
@@ -598,37 +607,38 @@
         <v>29</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4" s="6">
+        <v>30</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" s="6">
         <v>39.99</v>
       </c>
-      <c r="T4" s="6">
+      <c r="U4" s="6">
         <v>55.83</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B5" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
+        <v>43693</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
-      <c r="E5" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>25</v>
+      <c r="E5" s="6"/>
+      <c r="F5" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>28</v>
@@ -639,32 +649,33 @@
       <c r="K5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="L5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R5" s="6">
         <v>14.5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B6" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
+        <v>43693</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
-      <c r="E6" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>25</v>
+      <c r="E6" s="6"/>
+      <c r="F6" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>28</v>
@@ -675,32 +686,33 @@
       <c r="K6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q6" s="6">
+      <c r="L6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R6" s="6">
         <v>20.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B7" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
+        <v>43693</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>25</v>
+      <c r="E7" s="6"/>
+      <c r="F7" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>28</v>
@@ -709,34 +721,35 @@
         <v>29</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="R7" s="6">
+        <v>30</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="S7" s="6">
         <v>35.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B8" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
+        <v>43693</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>25</v>
+      <c r="E8" s="6"/>
+      <c r="F8" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>28</v>
@@ -747,32 +760,33 @@
       <c r="K8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q8" s="6">
+      <c r="L8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R8" s="6">
         <v>7.5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B9" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
+        <v>43693</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>25</v>
+      <c r="E9" s="6"/>
+      <c r="F9" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>28</v>
@@ -783,32 +797,33 @@
       <c r="K9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q9" s="6">
+      <c r="L9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R9" s="6">
         <v>35.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B10" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
+        <v>43693</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>25</v>
+      <c r="E10" s="6"/>
+      <c r="F10" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>28</v>
@@ -819,34 +834,35 @@
       <c r="K10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q10" s="6">
+      <c r="L10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R10" s="6">
         <v>15.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B11" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="12" t="s">
+        <v>43693</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>25</v>
+      <c r="E11" s="6"/>
+      <c r="F11" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>28</v>
@@ -857,34 +873,35 @@
       <c r="K11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q11" s="6">
+      <c r="L11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R11" s="6">
         <v>25.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B12" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>25</v>
+        <v>43693</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>28</v>
@@ -895,34 +912,35 @@
       <c r="K12" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q12" s="6">
+      <c r="L12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R12" s="6">
         <v>25.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B13" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>25</v>
+        <v>43693</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>28</v>
@@ -933,34 +951,35 @@
       <c r="K13" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q13" s="6">
+      <c r="L13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R13" s="6">
         <v>25.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B14" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>25</v>
+        <v>43693</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>28</v>
@@ -971,34 +990,35 @@
       <c r="K14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q14" s="6">
+      <c r="L14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R14" s="6">
         <v>25.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B15" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>25</v>
+        <v>43693</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>28</v>
@@ -1009,35 +1029,36 @@
       <c r="K15" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q15" s="6">
+      <c r="L15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R15" s="6">
         <v>25.0</v>
       </c>
-      <c r="R15" s="14"/>
+      <c r="S15" s="15"/>
     </row>
     <row r="16">
       <c r="A16" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B16" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>25</v>
+        <v>43693</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>28</v>
@@ -1048,34 +1069,35 @@
       <c r="K16" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q16" s="6">
+      <c r="L16" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R16" s="6">
         <v>25.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B17" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>25</v>
+        <v>43693</v>
+      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>28</v>
@@ -1086,34 +1108,35 @@
       <c r="K17" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q17" s="6">
+      <c r="L17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R17" s="6">
         <v>25.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B18" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>25</v>
+        <v>43693</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>28</v>
@@ -1124,34 +1147,35 @@
       <c r="K18" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q18" s="6">
+      <c r="L18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R18" s="6">
         <v>25.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B19" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>25</v>
+        <v>43693</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="I19" s="6" t="s">
         <v>28</v>
@@ -1162,34 +1186,35 @@
       <c r="K19" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q19" s="6">
+      <c r="L19" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R19" s="6">
         <v>25.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B20" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>25</v>
+        <v>43693</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="I20" s="6" t="s">
         <v>28</v>
@@ -1200,34 +1225,35 @@
       <c r="K20" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q20" s="6">
+      <c r="L20" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R20" s="6">
         <v>25.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B21" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>25</v>
+        <v>43693</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>28</v>
@@ -1238,34 +1264,35 @@
       <c r="K21" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q21" s="6">
+      <c r="L21" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R21" s="6">
         <v>25.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B22" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>25</v>
+        <v>43693</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="6"/>
+      <c r="F22" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>28</v>
@@ -1276,34 +1303,35 @@
       <c r="K22" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q22" s="6">
+      <c r="L22" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R22" s="6">
         <v>25.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B23" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>25</v>
+        <v>43693</v>
+      </c>
+      <c r="C23" s="11"/>
+      <c r="D23" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>28</v>
@@ -1314,34 +1342,35 @@
       <c r="K23" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q23" s="6">
+      <c r="L23" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R23" s="6">
         <v>25.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B24" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>25</v>
+        <v>43693</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="6"/>
+      <c r="F24" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>28</v>
@@ -1352,34 +1381,35 @@
       <c r="K24" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q24" s="6">
+      <c r="L24" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R24" s="6">
         <v>25.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B25" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>25</v>
+        <v>43693</v>
+      </c>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="6"/>
+      <c r="F25" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>28</v>
@@ -1390,34 +1420,35 @@
       <c r="K25" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q25" s="6">
+      <c r="L25" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R25" s="6">
         <v>25.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B26" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>25</v>
+        <v>43693</v>
+      </c>
+      <c r="C26" s="11"/>
+      <c r="D26" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26" s="6"/>
+      <c r="F26" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="I26" s="6" t="s">
         <v>28</v>
@@ -1428,34 +1459,35 @@
       <c r="K26" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q26" s="6">
+      <c r="L26" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R26" s="6">
         <v>25.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B27" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>25</v>
+        <v>43693</v>
+      </c>
+      <c r="C27" s="11"/>
+      <c r="D27" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="I27" s="6" t="s">
         <v>28</v>
@@ -1466,34 +1498,35 @@
       <c r="K27" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q27" s="6">
+      <c r="L27" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R27" s="6">
         <v>25.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B28" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>25</v>
+        <v>43693</v>
+      </c>
+      <c r="C28" s="11"/>
+      <c r="D28" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="I28" s="6" t="s">
         <v>28</v>
@@ -1504,34 +1537,35 @@
       <c r="K28" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q28" s="6">
+      <c r="L28" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R28" s="6">
         <v>25.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B29" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>25</v>
+        <v>43693</v>
+      </c>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="6"/>
+      <c r="F29" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="I29" s="6" t="s">
         <v>28</v>
@@ -1542,34 +1576,35 @@
       <c r="K29" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q29" s="6">
+      <c r="L29" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R29" s="6">
         <v>5.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B30" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>25</v>
+        <v>43693</v>
+      </c>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30" s="6"/>
+      <c r="F30" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="I30" s="6" t="s">
         <v>28</v>
@@ -1580,34 +1615,35 @@
       <c r="K30" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q30" s="6">
+      <c r="L30" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R30" s="6">
         <v>5.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B31" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>25</v>
+        <v>43693</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" s="6"/>
+      <c r="F31" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="I31" s="6" t="s">
         <v>28</v>
@@ -1618,34 +1654,35 @@
       <c r="K31" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q31" s="6">
+      <c r="L31" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R31" s="6">
         <v>5.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B32" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="D32" s="6"/>
-      <c r="E32" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>25</v>
+        <v>43693</v>
+      </c>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" s="6"/>
+      <c r="F32" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="I32" s="6" t="s">
         <v>28</v>
@@ -1656,34 +1693,35 @@
       <c r="K32" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q32" s="6">
+      <c r="L32" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R32" s="6">
         <v>5.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B33" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>25</v>
+        <v>43693</v>
+      </c>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="E33" s="6"/>
+      <c r="F33" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="I33" s="6" t="s">
         <v>28</v>
@@ -1694,34 +1732,35 @@
       <c r="K33" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q33" s="6">
+      <c r="L33" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R33" s="6">
         <v>5.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B34" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="D34" s="6"/>
-      <c r="E34" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>25</v>
+        <v>43693</v>
+      </c>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" s="6"/>
+      <c r="F34" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="I34" s="6" t="s">
         <v>28</v>
@@ -1732,30 +1771,30 @@
       <c r="K34" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q34" s="6">
+      <c r="L34" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R34" s="6">
         <v>5.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B35" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G35" s="16" t="s">
+        <v>43693</v>
+      </c>
+      <c r="F35" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="H35" s="6" t="s">
-        <v>27</v>
+      <c r="G35" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H35" s="17" t="s">
+        <v>35</v>
       </c>
       <c r="I35" s="6" t="s">
         <v>28</v>
@@ -1764,38 +1803,38 @@
         <v>29</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L35" s="6">
+        <v>30</v>
+      </c>
+      <c r="L35" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M35" s="6">
         <v>54.4</v>
       </c>
-      <c r="T35" s="6">
+      <c r="U35" s="6">
         <v>55.83</v>
       </c>
-      <c r="X35" s="6" t="b">
+      <c r="Y35" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B36" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G36" s="17" t="s">
+        <v>43693</v>
+      </c>
+      <c r="F36" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="H36" s="6" t="s">
-        <v>27</v>
+      <c r="G36" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H36" s="18" t="s">
+        <v>77</v>
       </c>
       <c r="I36" s="6" t="s">
         <v>28</v>
@@ -1806,33 +1845,33 @@
       <c r="K36" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q36" s="6">
+      <c r="L36" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R36" s="6">
         <v>40.0</v>
       </c>
-      <c r="X36" s="6" t="b">
+      <c r="Y36" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="5">
         <f t="shared" si="1"/>
-        <v>43307</v>
+        <v>43328</v>
       </c>
       <c r="B37" s="5">
         <f t="shared" si="2"/>
-        <v>43672</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G37" s="17" t="s">
+        <v>43693</v>
+      </c>
+      <c r="F37" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="H37" s="6" t="s">
-        <v>27</v>
+      <c r="G37" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H37" s="18" t="s">
+        <v>79</v>
       </c>
       <c r="I37" s="6" t="s">
         <v>28</v>
@@ -1841,15 +1880,18 @@
         <v>29</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="P37" s="6">
+        <v>30</v>
+      </c>
+      <c r="L37" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q37" s="6">
         <v>3.0</v>
       </c>
-      <c r="T37" s="6">
+      <c r="U37" s="6">
         <v>9.0</v>
       </c>
-      <c r="X37" s="6" t="b">
+      <c r="Y37" s="6" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>